<commit_message>
Carra pushing the latest changes to the code
</commit_message>
<xml_diff>
--- a/Dreissenid_Mussel_Model/Results/Test_Sensitivity_Results.xlsx
+++ b/Dreissenid_Mussel_Model/Results/Test_Sensitivity_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RDEL1CMC\Desktop\Congressional_Ad_Projects\Dreissenid_Mussel_Model\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6471026E-7744-42F7-868A-FE0ADFB4F6A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672FC8DD-3E4D-498A-A522-EF659B623BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4170" yWindow="3255" windowWidth="21600" windowHeight="11385" xr2:uid="{291201D8-3B18-4629-8F50-6E0AB0A37D78}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{291201D8-3B18-4629-8F50-6E0AB0A37D78}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,13 +48,13 @@
     <t>RunNumber</t>
   </si>
   <si>
-    <t>null boat threshold 50</t>
+    <t>HSI 20% decrease</t>
   </si>
   <si>
-    <t>null boat threshold 100</t>
+    <t>HSI Neutral</t>
   </si>
   <si>
-    <t>null boat threshold 1000</t>
+    <t>HSO 20% increase</t>
   </si>
 </sst>
 </file>
@@ -70,7 +70,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -80,12 +80,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -103,7 +97,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -120,13 +126,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9504A23F-A1BB-4443-A3EF-43ABD2F491DE}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,10 +477,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="2">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C2">
@@ -484,94 +491,94 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="2">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3">
-        <v>115</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" s="2">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4">
-        <v>215</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="A5" s="2">
+        <v>6</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5">
-        <v>261</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="A6" s="2">
+        <v>6</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6">
-        <v>303</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7">
-        <v>316</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8">
-        <v>317</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <v>2</v>
-      </c>
-      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C9">
@@ -583,96 +590,96 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <v>2</v>
-      </c>
-      <c r="B10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10">
-        <v>76</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <v>2</v>
-      </c>
-      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C11">
         <v>3</v>
       </c>
       <c r="D11">
-        <v>148</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <v>2</v>
-      </c>
-      <c r="B12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C12">
         <v>4</v>
       </c>
       <c r="D12">
-        <v>173</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="4"/>
+        <v>114</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="3"/>
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>2</v>
-      </c>
-      <c r="B13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C13">
         <v>5</v>
       </c>
       <c r="D13">
-        <v>188</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>2</v>
-      </c>
-      <c r="B14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C14">
         <v>6</v>
       </c>
       <c r="D14">
-        <v>193</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <v>2</v>
-      </c>
-      <c r="B15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C15">
         <v>7</v>
       </c>
       <c r="D15">
-        <v>199</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>5</v>
-      </c>
-      <c r="B16" s="2" t="s">
+      <c r="A16" s="6">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
         <v>6</v>
       </c>
       <c r="C16">
@@ -683,87 +690,87 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>5</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="A17" s="6">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
         <v>6</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
       <c r="D17">
-        <v>20</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>5</v>
-      </c>
-      <c r="B18" s="2" t="s">
+      <c r="A18" s="6">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="C18">
         <v>3</v>
       </c>
       <c r="D18">
-        <v>26</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>5</v>
-      </c>
-      <c r="B19" s="2" t="s">
+      <c r="A19" s="6">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
         <v>6</v>
       </c>
       <c r="C19">
         <v>4</v>
       </c>
       <c r="D19">
-        <v>26</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>5</v>
-      </c>
-      <c r="B20" s="2" t="s">
+      <c r="A20" s="6">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
         <v>6</v>
       </c>
       <c r="C20">
         <v>5</v>
       </c>
       <c r="D20">
-        <v>26</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <v>5</v>
-      </c>
-      <c r="B21" s="2" t="s">
+      <c r="A21" s="6">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
         <v>6</v>
       </c>
       <c r="C21">
         <v>6</v>
       </c>
       <c r="D21">
-        <v>26</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>5</v>
-      </c>
-      <c r="B22" s="2" t="s">
+      <c r="A22" s="6">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
         <v>6</v>
       </c>
       <c r="C22">
         <v>7</v>
       </c>
       <c r="D22">
-        <v>26</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>